<commit_message>
updated script, data files for state granualrity of output file
</commit_message>
<xml_diff>
--- a/data/nass_usda.xlsx
+++ b/data/nass_usda.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendallkikkawa/Documents/BAPP/GFI_rancher/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendallkikkawa/Documents/BAPP/GFI_rancher_project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763EC942-CAB6-3242-904A-2441113A6564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A37748-5EC7-6946-95CB-A18F5A6F62B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{43802369-0049-F641-A0B4-406613CA3578}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Number of Family Farmers</t>
-  </si>
-  <si>
     <t>United States</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>Wyoming</t>
+  </si>
+  <si>
+    <t>Number_of_Family_Farmers</t>
   </si>
 </sst>
 </file>
@@ -573,7 +573,7 @@
   <dimension ref="A1:E103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -591,12 +591,12 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2">
         <v>2017</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>2017</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="4" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>2017</v>
@@ -630,7 +630,7 @@
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>2017</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>2017</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
         <v>2017</v>
@@ -663,7 +663,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>2017</v>
@@ -674,7 +674,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2">
         <v>2017</v>
@@ -685,7 +685,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2">
         <v>2017</v>
@@ -696,7 +696,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2">
         <v>2017</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2">
         <v>2017</v>
@@ -718,7 +718,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2">
         <v>2017</v>
@@ -729,7 +729,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="2">
         <v>2017</v>
@@ -740,7 +740,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2">
         <v>2017</v>
@@ -751,7 +751,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2">
         <v>2017</v>
@@ -762,7 +762,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2">
         <v>2017</v>
@@ -773,7 +773,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="2">
         <v>2017</v>
@@ -784,7 +784,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="2">
         <v>2017</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="2">
         <v>2017</v>
@@ -806,7 +806,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="2">
         <v>2017</v>
@@ -817,7 +817,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="2">
         <v>2017</v>
@@ -828,7 +828,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="2">
         <v>2017</v>
@@ -839,7 +839,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="2">
         <v>2017</v>
@@ -850,7 +850,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="2">
         <v>2017</v>
@@ -861,7 +861,7 @@
     </row>
     <row r="26" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="2">
         <v>2017</v>
@@ -872,7 +872,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="2">
         <v>2017</v>
@@ -883,7 +883,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="2">
         <v>2017</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="2">
         <v>2017</v>
@@ -905,7 +905,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="2">
         <v>2017</v>
@@ -916,7 +916,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="2">
         <v>2017</v>
@@ -927,7 +927,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="2">
         <v>2017</v>
@@ -938,7 +938,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="2">
         <v>2017</v>
@@ -949,7 +949,7 @@
     </row>
     <row r="34" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" s="2">
         <v>2017</v>
@@ -960,7 +960,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" s="2">
         <v>2017</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" s="2">
         <v>2017</v>
@@ -982,7 +982,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" s="2">
         <v>2017</v>
@@ -993,7 +993,7 @@
     </row>
     <row r="38" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" s="2">
         <v>2017</v>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="39" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" s="2">
         <v>2017</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" s="2">
         <v>2017</v>
@@ -1026,7 +1026,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="2">
         <v>2017</v>
@@ -1037,7 +1037,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" s="2">
         <v>2017</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="43" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" s="2">
         <v>2017</v>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="44" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" s="2">
         <v>2017</v>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="45" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" s="2">
         <v>2017</v>
@@ -1081,7 +1081,7 @@
     </row>
     <row r="46" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46" s="2">
         <v>2017</v>
@@ -1092,7 +1092,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" s="2">
         <v>2017</v>
@@ -1103,7 +1103,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48" s="2">
         <v>2017</v>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49" s="2">
         <v>2017</v>
@@ -1125,7 +1125,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50" s="2">
         <v>2017</v>
@@ -1136,7 +1136,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51" s="2">
         <v>2017</v>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" s="2">
         <v>2017</v>
@@ -1158,7 +1158,7 @@
     </row>
     <row r="53" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B53" s="2">
         <v>2012</v>
@@ -1170,7 +1170,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B54" s="2">
         <v>2012</v>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B55" s="2">
         <v>2012</v>
@@ -1192,7 +1192,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B56" s="2">
         <v>2012</v>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B57" s="2">
         <v>2012</v>
@@ -1214,7 +1214,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B58" s="2">
         <v>2012</v>
@@ -1225,7 +1225,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B59" s="2">
         <v>2012</v>
@@ -1236,7 +1236,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B60" s="2">
         <v>2012</v>
@@ -1247,7 +1247,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B61" s="2">
         <v>2012</v>
@@ -1258,7 +1258,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B62" s="2">
         <v>2012</v>
@@ -1269,7 +1269,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B63" s="2">
         <v>2012</v>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B64" s="2">
         <v>2012</v>
@@ -1291,7 +1291,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B65" s="2">
         <v>2012</v>
@@ -1302,7 +1302,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B66" s="2">
         <v>2012</v>
@@ -1313,7 +1313,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B67" s="2">
         <v>2012</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B68" s="2">
         <v>2012</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B69" s="2">
         <v>2012</v>
@@ -1346,7 +1346,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B70" s="2">
         <v>2012</v>
@@ -1357,7 +1357,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B71" s="2">
         <v>2012</v>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B72" s="2">
         <v>2012</v>
@@ -1379,7 +1379,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B73" s="2">
         <v>2012</v>
@@ -1390,7 +1390,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B74" s="2">
         <v>2012</v>
@@ -1401,7 +1401,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B75" s="2">
         <v>2012</v>
@@ -1412,7 +1412,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B76" s="2">
         <v>2012</v>
@@ -1423,7 +1423,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B77" s="2">
         <v>2012</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B78" s="2">
         <v>2012</v>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B79" s="2">
         <v>2012</v>
@@ -1456,7 +1456,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B80" s="2">
         <v>2012</v>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B81" s="2">
         <v>2012</v>
@@ -1478,7 +1478,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B82" s="2">
         <v>2012</v>
@@ -1489,7 +1489,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B83" s="2">
         <v>2012</v>
@@ -1500,7 +1500,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B84" s="2">
         <v>2012</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B85" s="2">
         <v>2012</v>
@@ -1522,7 +1522,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B86" s="2">
         <v>2012</v>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B87" s="2">
         <v>2012</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B88" s="2">
         <v>2012</v>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B89" s="2">
         <v>2012</v>
@@ -1566,7 +1566,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B90" s="2">
         <v>2012</v>
@@ -1577,7 +1577,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B91" s="2">
         <v>2012</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B92" s="2">
         <v>2012</v>
@@ -1599,7 +1599,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B93" s="2">
         <v>2012</v>
@@ -1610,7 +1610,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B94" s="2">
         <v>2012</v>
@@ -1621,7 +1621,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B95" s="2">
         <v>2012</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B96" s="2">
         <v>2012</v>
@@ -1643,7 +1643,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B97" s="2">
         <v>2012</v>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B98" s="2">
         <v>2012</v>
@@ -1665,7 +1665,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B99" s="2">
         <v>2012</v>
@@ -1676,7 +1676,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B100" s="2">
         <v>2012</v>
@@ -1687,7 +1687,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B101" s="2">
         <v>2012</v>
@@ -1698,7 +1698,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B102" s="2">
         <v>2012</v>
@@ -1709,7 +1709,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B103" s="2">
         <v>2012</v>

</xml_diff>